<commit_message>
Innan lottning sm 2023
</commit_message>
<xml_diff>
--- a/mallar/import/sm_nm 2023/extraktion_01-SMNM2023 - med NM - v230705.xlsx
+++ b/mallar/import/sm_nm 2023/extraktion_01-SMNM2023 - med NM - v230705.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\episerver\voltige\VoltigeClosedXML\mallar\import\sm_nm 2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{092C4F4F-3DA3-4A21-8DE1-E465E278959C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ACCA607-F9F6-4E9D-AECA-9E759CC29278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" tabRatio="483" xr2:uid="{9C6C5895-3CBC-495A-8EC3-24DF642F0EB2}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1206" uniqueCount="514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1210" uniqueCount="514">
   <si>
     <t>Linda Jenvall</t>
   </si>
@@ -1002,9 +1002,6 @@
   </si>
   <si>
     <t>Linnea, Amalia Glimmerhav, Edla Danielsson, Anna-Liisa Anson</t>
-  </si>
-  <si>
-    <t>Heitti Räisänen</t>
   </si>
   <si>
     <t>Gold 2</t>
@@ -1599,6 +1596,9 @@
   </si>
   <si>
     <t>Pas de deux NM 2*</t>
+  </si>
+  <si>
+    <t>VCF</t>
   </si>
 </sst>
 </file>
@@ -2004,8 +2004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73B3B0E3-2027-4083-B582-AAB0C4C3F786}">
   <dimension ref="A1:W110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView tabSelected="1" topLeftCell="G93" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H108" sqref="H108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2127,7 +2127,7 @@
         <v>2</v>
       </c>
       <c r="J2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="K2" t="s">
         <v>183</v>
@@ -2189,7 +2189,7 @@
         <v>301477</v>
       </c>
       <c r="G3" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H3">
         <v>223</v>
@@ -2337,7 +2337,7 @@
         <v>48</v>
       </c>
       <c r="J5" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="K5" t="s">
         <v>186</v>
@@ -2479,7 +2479,7 @@
         <v>167</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="K7" s="4" t="s">
         <v>188</v>
@@ -2621,7 +2621,7 @@
         <v>29</v>
       </c>
       <c r="J9" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L9">
         <v>131893</v>
@@ -2659,7 +2659,7 @@
         <v>29</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L10">
         <v>35251</v>
@@ -2697,7 +2697,7 @@
         <v>9</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="L11">
         <v>40406</v>
@@ -2735,7 +2735,7 @@
         <v>12</v>
       </c>
       <c r="J12" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="L12">
         <v>145535</v>
@@ -2773,7 +2773,7 @@
         <v>12</v>
       </c>
       <c r="J13" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="L13">
         <v>106236</v>
@@ -2963,7 +2963,7 @@
         <v>9</v>
       </c>
       <c r="J18" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="L18">
         <v>124198</v>
@@ -3036,7 +3036,7 @@
         <v>29</v>
       </c>
       <c r="J20" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="L20">
         <v>60750</v>
@@ -3138,7 +3138,7 @@
         <v>200293760</v>
       </c>
       <c r="G23" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="H23">
         <v>869</v>
@@ -3147,7 +3147,7 @@
         <v>12</v>
       </c>
       <c r="J23" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="L23">
         <v>120827</v>
@@ -3176,7 +3176,7 @@
         <v>200293760</v>
       </c>
       <c r="G24" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="H24">
         <v>223</v>
@@ -3185,7 +3185,7 @@
         <v>2</v>
       </c>
       <c r="J24" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="L24">
         <v>69830</v>
@@ -3223,7 +3223,7 @@
         <v>48</v>
       </c>
       <c r="J25" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="L25">
         <v>129688</v>
@@ -3261,7 +3261,7 @@
         <v>48</v>
       </c>
       <c r="J26" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="L26">
         <v>107961</v>
@@ -3299,7 +3299,7 @@
         <v>48</v>
       </c>
       <c r="J27" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="L27">
         <v>108087</v>
@@ -3337,7 +3337,7 @@
         <v>48</v>
       </c>
       <c r="J28" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="L28">
         <v>134138</v>
@@ -3375,7 +3375,7 @@
         <v>2</v>
       </c>
       <c r="J29" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="L29">
         <v>74165</v>
@@ -3413,7 +3413,7 @@
         <v>2</v>
       </c>
       <c r="J30" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="L30">
         <v>101580</v>
@@ -3451,7 +3451,7 @@
         <v>2</v>
       </c>
       <c r="J31" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="L31">
         <v>101407</v>
@@ -3527,7 +3527,7 @@
         <v>2</v>
       </c>
       <c r="J33" s="9" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="L33">
         <v>145224</v>
@@ -3565,7 +3565,7 @@
         <v>2</v>
       </c>
       <c r="J34" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="L34">
         <v>109403</v>
@@ -3603,7 +3603,7 @@
         <v>29</v>
       </c>
       <c r="J35" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="L35">
         <v>130120</v>
@@ -3641,7 +3641,7 @@
         <v>29</v>
       </c>
       <c r="J36" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="L36">
         <v>87139</v>
@@ -3717,7 +3717,7 @@
         <v>2</v>
       </c>
       <c r="J38" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="L38">
         <v>149851</v>
@@ -3793,7 +3793,7 @@
         <v>12</v>
       </c>
       <c r="J40" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="L40">
         <v>162160</v>
@@ -3831,7 +3831,7 @@
         <v>173</v>
       </c>
       <c r="J41" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="L41">
         <v>166499</v>
@@ -3869,7 +3869,7 @@
         <v>55</v>
       </c>
       <c r="J42" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="L42">
         <v>51513</v>
@@ -3907,7 +3907,7 @@
         <v>55</v>
       </c>
       <c r="J43" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="L43">
         <v>164089</v>
@@ -3945,7 +3945,7 @@
         <v>2</v>
       </c>
       <c r="J44" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="L44">
         <v>150091</v>
@@ -4021,7 +4021,7 @@
         <v>167</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="L46">
         <v>152057</v>
@@ -4059,7 +4059,7 @@
         <v>167</v>
       </c>
       <c r="J47" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="L47">
         <v>164002</v>
@@ -4097,7 +4097,7 @@
         <v>167</v>
       </c>
       <c r="J48" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="L48" s="4">
         <v>160046</v>
@@ -4135,7 +4135,7 @@
         <v>172</v>
       </c>
       <c r="J49" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="L49">
         <v>123786</v>
@@ -4173,7 +4173,7 @@
         <v>55</v>
       </c>
       <c r="J50" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="L50">
         <v>50023</v>
@@ -4328,7 +4328,7 @@
         <v>2</v>
       </c>
       <c r="J54" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="K54" t="s">
         <v>191</v>
@@ -4375,16 +4375,16 @@
         <v>173</v>
       </c>
       <c r="J55" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="K55" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="L55">
         <v>103221</v>
       </c>
       <c r="M55" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="N55">
         <v>34693</v>
@@ -4422,7 +4422,7 @@
         <v>231</v>
       </c>
       <c r="J56" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="L56">
         <v>1001</v>
@@ -4460,7 +4460,7 @@
         <v>231</v>
       </c>
       <c r="J57" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="L57">
         <v>1002</v>
@@ -4498,7 +4498,7 @@
         <v>233</v>
       </c>
       <c r="J58" s="4" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="L58">
         <v>1003</v>
@@ -4536,7 +4536,7 @@
         <v>233</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="L59">
         <v>1005</v>
@@ -4641,10 +4641,10 @@
         <v>210</v>
       </c>
       <c r="I62" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="J62" s="5" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="L62">
         <v>1053</v>
@@ -4682,7 +4682,7 @@
         <v>234</v>
       </c>
       <c r="J63" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="L63">
         <v>1007</v>
@@ -4720,7 +4720,7 @@
         <v>231</v>
       </c>
       <c r="J64" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="L64">
         <v>1010</v>
@@ -4758,7 +4758,7 @@
         <v>231</v>
       </c>
       <c r="J65" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="L65">
         <v>1011</v>
@@ -4796,7 +4796,7 @@
         <v>231</v>
       </c>
       <c r="J66" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L66">
         <v>1012</v>
@@ -4834,7 +4834,7 @@
         <v>231</v>
       </c>
       <c r="J67" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="L67">
         <v>1013</v>
@@ -4908,7 +4908,7 @@
         <v>235</v>
       </c>
       <c r="J69" s="4" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="L69">
         <v>1014</v>
@@ -5042,7 +5042,7 @@
         <v>227</v>
       </c>
       <c r="F73">
-        <v>10</v>
+        <v>2000010</v>
       </c>
       <c r="G73" t="s">
         <v>209</v>
@@ -5080,7 +5080,7 @@
         <v>227</v>
       </c>
       <c r="F74">
-        <v>10</v>
+        <v>2000010</v>
       </c>
       <c r="G74" t="s">
         <v>209</v>
@@ -5127,7 +5127,7 @@
         <v>237</v>
       </c>
       <c r="J75" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="L75">
         <v>1020</v>
@@ -5165,7 +5165,7 @@
         <v>237</v>
       </c>
       <c r="J76" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="L76">
         <v>1021</v>
@@ -5191,7 +5191,7 @@
         <v>227</v>
       </c>
       <c r="F77">
-        <v>11</v>
+        <v>2000011</v>
       </c>
       <c r="G77" t="s">
         <v>210</v>
@@ -5203,7 +5203,7 @@
         <v>237</v>
       </c>
       <c r="J77" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="L77">
         <v>1022</v>
@@ -5229,7 +5229,7 @@
         <v>227</v>
       </c>
       <c r="F78">
-        <v>11</v>
+        <v>2000011</v>
       </c>
       <c r="G78" t="s">
         <v>210</v>
@@ -5241,7 +5241,7 @@
         <v>237</v>
       </c>
       <c r="J78" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="L78">
         <v>1023</v>
@@ -5422,7 +5422,7 @@
         <v>239</v>
       </c>
       <c r="J83" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="L83">
         <v>1029</v>
@@ -5460,7 +5460,7 @@
         <v>239</v>
       </c>
       <c r="J84" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="L84">
         <v>1030</v>
@@ -5492,7 +5492,7 @@
         <v>212</v>
       </c>
       <c r="H85">
-        <v>206</v>
+        <v>2000206</v>
       </c>
       <c r="I85" t="s">
         <v>239</v>
@@ -5545,7 +5545,7 @@
         <v>235</v>
       </c>
       <c r="J86" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="L86">
         <v>1032</v>
@@ -5583,7 +5583,7 @@
         <v>235</v>
       </c>
       <c r="J87" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="L87">
         <v>1033</v>
@@ -5694,7 +5694,7 @@
         <v>241</v>
       </c>
       <c r="J90" s="8" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="L90">
         <v>1040</v>
@@ -5803,7 +5803,7 @@
         <v>241</v>
       </c>
       <c r="J92" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="L92">
         <v>1039</v>
@@ -5841,7 +5841,7 @@
         <v>241</v>
       </c>
       <c r="J93" s="4" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="L93">
         <v>1038</v>
@@ -5870,7 +5870,7 @@
         <v>200000018</v>
       </c>
       <c r="G94" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="H94">
         <v>208</v>
@@ -5879,7 +5879,7 @@
         <v>241</v>
       </c>
       <c r="J94" s="4" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="L94">
         <v>1055</v>
@@ -5908,7 +5908,7 @@
         <v>200000018</v>
       </c>
       <c r="G95" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="H95">
         <v>208</v>
@@ -5943,7 +5943,7 @@
         <v>200000018</v>
       </c>
       <c r="G96" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="H96">
         <v>208</v>
@@ -5987,7 +5987,7 @@
         <v>241</v>
       </c>
       <c r="J97" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="L97">
         <v>1041</v>
@@ -6051,7 +6051,7 @@
         <v>21</v>
       </c>
       <c r="G99" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H99">
         <v>208</v>
@@ -6086,7 +6086,7 @@
         <v>21</v>
       </c>
       <c r="G100" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H100">
         <v>208</v>
@@ -6095,7 +6095,7 @@
         <v>241</v>
       </c>
       <c r="J100" s="4" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="L100">
         <v>1052</v>
@@ -6124,7 +6124,7 @@
         <v>21</v>
       </c>
       <c r="G101" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H101">
         <v>208</v>
@@ -6239,7 +6239,7 @@
         <v>241</v>
       </c>
       <c r="J103" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="L103">
         <v>1046</v>
@@ -6277,7 +6277,7 @@
         <v>241</v>
       </c>
       <c r="J104" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="L104">
         <v>1044</v>
@@ -6315,7 +6315,7 @@
         <v>180</v>
       </c>
       <c r="J105" s="3" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="L105" s="3">
         <v>95591</v>
@@ -6354,7 +6354,7 @@
         <v>180</v>
       </c>
       <c r="J106" s="3" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="L106" s="3">
         <v>112424</v>
@@ -6387,13 +6387,13 @@
         <v>122</v>
       </c>
       <c r="H107">
-        <v>669</v>
+        <v>772</v>
       </c>
       <c r="I107" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="J107" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="L107">
         <v>167975</v>
@@ -6422,7 +6422,7 @@
         <v>2000312178</v>
       </c>
       <c r="G108" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="H108" s="3">
         <v>594</v>
@@ -6431,7 +6431,7 @@
         <v>167</v>
       </c>
       <c r="J108" s="6" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="L108" s="3">
         <v>130283</v>
@@ -6461,7 +6461,7 @@
         <v>2000312178</v>
       </c>
       <c r="G109" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="H109">
         <v>594</v>
@@ -6470,7 +6470,7 @@
         <v>167</v>
       </c>
       <c r="J109" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="L109">
         <v>151413</v>
@@ -6499,7 +6499,7 @@
         <v>2000312178</v>
       </c>
       <c r="G110" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="H110">
         <v>594</v>
@@ -6508,7 +6508,7 @@
         <v>167</v>
       </c>
       <c r="J110" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="L110">
         <v>177919</v>
@@ -6545,7 +6545,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
@@ -6556,7 +6556,7 @@
         <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D2">
         <v>4</v>
@@ -6576,7 +6576,7 @@
         <v>135</v>
       </c>
       <c r="C3" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="D3">
         <v>4</v>
@@ -6593,7 +6593,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D4">
         <v>16</v>
@@ -6610,7 +6610,7 @@
         <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="D5">
         <v>16</v>
@@ -6630,7 +6630,7 @@
         <v>139</v>
       </c>
       <c r="C6" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D6">
         <v>16</v>
@@ -6647,7 +6647,7 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
@@ -6658,7 +6658,7 @@
         <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D8">
         <v>26</v>
@@ -6695,7 +6695,7 @@
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
@@ -6706,7 +6706,7 @@
         <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="D11">
         <v>1061</v>
@@ -6743,7 +6743,7 @@
         <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
@@ -6754,7 +6754,7 @@
         <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D14">
         <v>1079</v>
@@ -6791,7 +6791,7 @@
         <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D16">
         <v>1080</v>
@@ -6808,7 +6808,7 @@
         <v>26</v>
       </c>
       <c r="C17" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D17">
         <v>1080</v>
@@ -6828,7 +6828,7 @@
         <v>152</v>
       </c>
       <c r="C18" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D18">
         <v>1080</v>
@@ -6994,7 +6994,7 @@
         <v>18</v>
       </c>
       <c r="C29" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D29" s="5">
         <v>1091</v>
@@ -7011,7 +7011,7 @@
         <v>7</v>
       </c>
       <c r="C30" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
@@ -7022,7 +7022,7 @@
         <v>27</v>
       </c>
       <c r="C31" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
@@ -7050,7 +7050,7 @@
         <v>28</v>
       </c>
       <c r="C33" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D33">
         <v>1092</v>
@@ -7318,7 +7318,7 @@
         <v>111</v>
       </c>
       <c r="B30" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
   </sheetData>
@@ -7328,10 +7328,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E50BA4F-C9F6-4C5B-8947-232726082284}">
-  <dimension ref="A1:B52"/>
+  <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52:B52"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7721,7 +7721,7 @@
         <v>301477</v>
       </c>
       <c r="B48" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.45">
@@ -7729,7 +7729,7 @@
         <v>21</v>
       </c>
       <c r="B49" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.45">
@@ -7737,7 +7737,7 @@
         <v>200293760</v>
       </c>
       <c r="B50" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.45">
@@ -7745,7 +7745,7 @@
         <v>200000018</v>
       </c>
       <c r="B51" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.45">
@@ -7753,7 +7753,23 @@
         <v>2000312178</v>
       </c>
       <c r="B52" t="s">
-        <v>491</v>
+        <v>490</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A53">
+        <v>2000010</v>
+      </c>
+      <c r="B53" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A54">
+        <v>2000011</v>
+      </c>
+      <c r="B54" t="s">
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -7763,10 +7779,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9127C6F2-EC51-4670-8080-B1754AF093BC}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="A12" sqref="A12:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7989,7 +8005,7 @@
         <v>206</v>
       </c>
       <c r="B20" t="s">
-        <v>239</v>
+        <v>513</v>
       </c>
       <c r="C20" t="s">
         <v>236</v>
@@ -8033,10 +8049,21 @@
         <v>210</v>
       </c>
       <c r="B24" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C24" t="s">
         <v>292</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A25">
+        <v>2000206</v>
+      </c>
+      <c r="B25" t="s">
+        <v>239</v>
+      </c>
+      <c r="C25" t="s">
+        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -8048,8 +8075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D5152B9-B788-4BDE-A1B2-C618945E4F4F}">
   <dimension ref="A1:F137"/>
   <sheetViews>
-    <sheetView topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="B83" sqref="B83"/>
+    <sheetView topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="B110" sqref="B110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8114,7 +8141,7 @@
         <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
@@ -8125,7 +8152,7 @@
         <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
@@ -8136,7 +8163,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
@@ -8147,7 +8174,7 @@
         <v>45</v>
       </c>
       <c r="C10" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
@@ -8158,7 +8185,7 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
@@ -8209,7 +8236,7 @@
         <v>34</v>
       </c>
       <c r="C17" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
@@ -8228,7 +8255,7 @@
         <v>3</v>
       </c>
       <c r="C19" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
@@ -8239,7 +8266,7 @@
         <v>5</v>
       </c>
       <c r="C20" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.45">
@@ -8250,7 +8277,7 @@
         <v>4</v>
       </c>
       <c r="C21" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
@@ -8261,7 +8288,7 @@
         <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.45">
@@ -8272,7 +8299,7 @@
         <v>7</v>
       </c>
       <c r="C23" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.45">
@@ -8291,7 +8318,7 @@
         <v>35</v>
       </c>
       <c r="C25" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.45">
@@ -8302,7 +8329,7 @@
         <v>36</v>
       </c>
       <c r="C26" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.45">
@@ -8321,7 +8348,7 @@
         <v>38</v>
       </c>
       <c r="C28" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.45">
@@ -8332,7 +8359,7 @@
         <v>39</v>
       </c>
       <c r="C29" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.45">
@@ -8423,7 +8450,7 @@
         <v>78</v>
       </c>
       <c r="C40" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.45">
@@ -8434,7 +8461,7 @@
         <v>79</v>
       </c>
       <c r="C41" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.45">
@@ -8445,7 +8472,7 @@
         <v>80</v>
       </c>
       <c r="C42" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.45">
@@ -8456,7 +8483,7 @@
         <v>81</v>
       </c>
       <c r="C43" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.45">
@@ -8507,7 +8534,7 @@
         <v>87</v>
       </c>
       <c r="C49" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.45">
@@ -8518,7 +8545,7 @@
         <v>27</v>
       </c>
       <c r="C50" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.45">
@@ -8529,7 +8556,7 @@
         <v>47</v>
       </c>
       <c r="C51" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.45">
@@ -8540,7 +8567,7 @@
         <v>58</v>
       </c>
       <c r="C52" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.45">
@@ -8551,7 +8578,7 @@
         <v>28</v>
       </c>
       <c r="C53" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.45">
@@ -8562,7 +8589,7 @@
         <v>88</v>
       </c>
       <c r="C54" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.45">
@@ -8573,7 +8600,7 @@
         <v>89</v>
       </c>
       <c r="C55" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.45">
@@ -8584,7 +8611,7 @@
         <v>13</v>
       </c>
       <c r="C56" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.45">
@@ -8595,7 +8622,7 @@
         <v>16</v>
       </c>
       <c r="C57" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.45">
@@ -8606,7 +8633,7 @@
         <v>90</v>
       </c>
       <c r="C58" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.45">
@@ -8617,7 +8644,7 @@
         <v>91</v>
       </c>
       <c r="C59" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.45">
@@ -8628,7 +8655,7 @@
         <v>6</v>
       </c>
       <c r="C60" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.45">
@@ -8639,7 +8666,7 @@
         <v>46</v>
       </c>
       <c r="C61" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.45">
@@ -8650,7 +8677,7 @@
         <v>92</v>
       </c>
       <c r="C62" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.45">
@@ -8661,7 +8688,7 @@
         <v>93</v>
       </c>
       <c r="C63" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.45">
@@ -8672,7 +8699,7 @@
         <v>94</v>
       </c>
       <c r="C64" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.45">
@@ -8683,7 +8710,7 @@
         <v>95</v>
       </c>
       <c r="C65" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.45">
@@ -8694,7 +8721,7 @@
         <v>96</v>
       </c>
       <c r="C66" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.45">
@@ -8705,7 +8732,7 @@
         <v>59</v>
       </c>
       <c r="C67" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.45">
@@ -8716,7 +8743,7 @@
         <v>97</v>
       </c>
       <c r="C68" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.45">
@@ -8727,7 +8754,7 @@
         <v>98</v>
       </c>
       <c r="C69" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.45">
@@ -8738,7 +8765,7 @@
         <v>99</v>
       </c>
       <c r="C70" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.45">
@@ -8749,7 +8776,7 @@
         <v>65</v>
       </c>
       <c r="C71" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.45">
@@ -8760,7 +8787,7 @@
         <v>22</v>
       </c>
       <c r="C72" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.45">
@@ -8771,7 +8798,7 @@
         <v>100</v>
       </c>
       <c r="C73" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.45">
@@ -8782,7 +8809,7 @@
         <v>101</v>
       </c>
       <c r="C74" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.45">
@@ -8793,7 +8820,7 @@
         <v>102</v>
       </c>
       <c r="C75" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.45">
@@ -8804,7 +8831,7 @@
         <v>103</v>
       </c>
       <c r="C76" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.45">
@@ -8815,7 +8842,7 @@
         <v>104</v>
       </c>
       <c r="C77" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.45">
@@ -8826,7 +8853,7 @@
         <v>105</v>
       </c>
       <c r="C78" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.45">
@@ -8869,7 +8896,7 @@
         <v>244</v>
       </c>
       <c r="C83" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.45">
@@ -8880,7 +8907,7 @@
         <v>245</v>
       </c>
       <c r="C84" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.45">
@@ -8891,7 +8918,7 @@
         <v>246</v>
       </c>
       <c r="C85" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.45">
@@ -8902,7 +8929,7 @@
         <v>247</v>
       </c>
       <c r="C86" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.45">
@@ -8913,7 +8940,7 @@
         <v>248</v>
       </c>
       <c r="C87" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.45">
@@ -8924,7 +8951,7 @@
         <v>249</v>
       </c>
       <c r="C88" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.45">
@@ -8935,7 +8962,7 @@
         <v>250</v>
       </c>
       <c r="C89" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.45">
@@ -8954,7 +8981,7 @@
         <v>252</v>
       </c>
       <c r="C91" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.45">
@@ -8965,7 +8992,7 @@
         <v>253</v>
       </c>
       <c r="C92" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.45">
@@ -8976,7 +9003,7 @@
         <v>254</v>
       </c>
       <c r="C93" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.45">
@@ -8987,7 +9014,7 @@
         <v>255</v>
       </c>
       <c r="C94" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.45">
@@ -8998,7 +9025,7 @@
         <v>256</v>
       </c>
       <c r="C95" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.45">
@@ -9009,7 +9036,7 @@
         <v>257</v>
       </c>
       <c r="C96" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.45">
@@ -9020,7 +9047,7 @@
         <v>258</v>
       </c>
       <c r="C97" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.45">
@@ -9031,7 +9058,7 @@
         <v>259</v>
       </c>
       <c r="C98" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.45">
@@ -9042,7 +9069,7 @@
         <v>260</v>
       </c>
       <c r="C99" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.45">
@@ -9053,7 +9080,7 @@
         <v>261</v>
       </c>
       <c r="C100" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.45">
@@ -9061,10 +9088,10 @@
         <v>1019</v>
       </c>
       <c r="B101" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C101" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.45">
@@ -9075,7 +9102,7 @@
         <v>263</v>
       </c>
       <c r="C102" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.45">
@@ -9086,7 +9113,7 @@
         <v>264</v>
       </c>
       <c r="C103" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.45">
@@ -9097,7 +9124,7 @@
         <v>265</v>
       </c>
       <c r="C104" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.45">
@@ -9105,10 +9132,10 @@
         <v>1023</v>
       </c>
       <c r="B105" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C105" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.45">
@@ -9119,7 +9146,7 @@
         <v>267</v>
       </c>
       <c r="C106" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.45">
@@ -9130,7 +9157,7 @@
         <v>268</v>
       </c>
       <c r="C107" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.45">
@@ -9141,7 +9168,7 @@
         <v>269</v>
       </c>
       <c r="C108" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.45">
@@ -9149,10 +9176,10 @@
         <v>1027</v>
       </c>
       <c r="B109" t="s">
-        <v>321</v>
+        <v>270</v>
       </c>
       <c r="C109" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.45">
@@ -9171,7 +9198,7 @@
         <v>272</v>
       </c>
       <c r="C111" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.45">
@@ -9179,10 +9206,10 @@
         <v>1030</v>
       </c>
       <c r="B112" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C112" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.45">
@@ -9193,7 +9220,7 @@
         <v>275</v>
       </c>
       <c r="C113" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.45">
@@ -9204,7 +9231,7 @@
         <v>276</v>
       </c>
       <c r="C114" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.45">
@@ -9215,7 +9242,7 @@
         <v>278</v>
       </c>
       <c r="C115" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.45">
@@ -9226,7 +9253,7 @@
         <v>279</v>
       </c>
       <c r="C116" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.45">
@@ -9237,7 +9264,7 @@
         <v>281</v>
       </c>
       <c r="C117" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.45">
@@ -9248,7 +9275,7 @@
         <v>282</v>
       </c>
       <c r="C118" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.45">
@@ -9259,7 +9286,7 @@
         <v>283</v>
       </c>
       <c r="C119" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.45">
@@ -9270,7 +9297,7 @@
         <v>284</v>
       </c>
       <c r="C120" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.45">
@@ -9281,7 +9308,7 @@
         <v>285</v>
       </c>
       <c r="C121" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.45">
@@ -9292,7 +9319,7 @@
         <v>286</v>
       </c>
       <c r="C122" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F122" s="4"/>
     </row>
@@ -9304,7 +9331,7 @@
         <v>287</v>
       </c>
       <c r="C123" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.45">
@@ -9315,7 +9342,7 @@
         <v>289</v>
       </c>
       <c r="C124" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.45">
@@ -9326,7 +9353,7 @@
         <v>290</v>
       </c>
       <c r="C125" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.45">
@@ -9337,7 +9364,7 @@
         <v>291</v>
       </c>
       <c r="C126" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.45">
@@ -9372,7 +9399,7 @@
         <v>302</v>
       </c>
       <c r="C130" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.45">
@@ -9383,7 +9410,7 @@
         <v>304</v>
       </c>
       <c r="C131" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.45">
@@ -9394,7 +9421,7 @@
         <v>315</v>
       </c>
       <c r="C132" s="6" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.45">
@@ -9405,7 +9432,7 @@
         <v>316</v>
       </c>
       <c r="C133" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.45">
@@ -9416,7 +9443,7 @@
         <v>317</v>
       </c>
       <c r="C134" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.45">
@@ -9427,7 +9454,7 @@
         <v>318</v>
       </c>
       <c r="C135" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.45">
@@ -9438,7 +9465,7 @@
         <v>319</v>
       </c>
       <c r="C136" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.45">
@@ -9449,7 +9476,7 @@
         <v>277</v>
       </c>
       <c r="C137" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
   </sheetData>
@@ -9480,7 +9507,7 @@
         <v>301477</v>
       </c>
       <c r="B2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
@@ -9512,7 +9539,7 @@
         <v>266295</v>
       </c>
       <c r="B6" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
@@ -9520,7 +9547,7 @@
         <v>265064</v>
       </c>
       <c r="B7" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">

</xml_diff>